<commit_message>
Data feeds adjusted to new root region concordance.
</commit_message>
<xml_diff>
--- a/ConcordanceLibrary/LabelsAndCodes/PIOLab_RootClassification.xlsx
+++ b/ConcordanceLibrary/LabelsAndCodes/PIOLab_RootClassification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="819" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="819"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="1039">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -3145,6 +3145,9 @@
   </si>
   <si>
     <t>ZZZZ</t>
+  </si>
+  <si>
+    <t>ISONum3</t>
   </si>
 </sst>
 </file>
@@ -3512,8 +3515,8 @@
   </sheetPr>
   <dimension ref="A1:Z245"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3541,6 +3544,9 @@
       <c r="E1" s="1" t="s">
         <v>943</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>1038</v>
+      </c>
       <c r="Z1" s="8"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
@@ -3559,6 +3565,9 @@
       <c r="E2" t="s">
         <v>1037</v>
       </c>
+      <c r="F2">
+        <v>533</v>
+      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -3576,6 +3585,9 @@
       <c r="E3" t="s">
         <v>539</v>
       </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -3593,6 +3605,9 @@
       <c r="E4" t="s">
         <v>547</v>
       </c>
+      <c r="F4">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -3610,6 +3625,9 @@
       <c r="E5" t="s">
         <v>1037</v>
       </c>
+      <c r="F5">
+        <v>660</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -3627,6 +3645,9 @@
       <c r="E6" t="s">
         <v>541</v>
       </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -3644,6 +3665,9 @@
       <c r="E7" t="s">
         <v>545</v>
       </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -3661,6 +3685,9 @@
       <c r="E8" t="s">
         <v>1037</v>
       </c>
+      <c r="F8">
+        <v>530</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -3678,6 +3705,9 @@
       <c r="E9" t="s">
         <v>901</v>
       </c>
+      <c r="F9">
+        <v>784</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -3695,6 +3725,9 @@
       <c r="E10" t="s">
         <v>553</v>
       </c>
+      <c r="F10">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -3712,6 +3745,9 @@
       <c r="E11" t="s">
         <v>565</v>
       </c>
+      <c r="F11">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -3729,6 +3765,9 @@
       <c r="E12" t="s">
         <v>549</v>
       </c>
+      <c r="F12">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -3746,6 +3785,9 @@
       <c r="E13" t="s">
         <v>555</v>
       </c>
+      <c r="F13">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -3763,6 +3805,9 @@
       <c r="E14" t="s">
         <v>557</v>
       </c>
+      <c r="F14">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -3780,6 +3825,9 @@
       <c r="E15" t="s">
         <v>551</v>
       </c>
+      <c r="F15">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -3797,8 +3845,11 @@
       <c r="E16" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3814,8 +3865,11 @@
       <c r="E17" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3831,8 +3885,11 @@
       <c r="E18" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3848,8 +3905,11 @@
       <c r="E19" t="s">
         <v>926</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3865,8 +3925,11 @@
       <c r="E20" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3882,8 +3945,11 @@
       <c r="E21" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3899,8 +3965,11 @@
       <c r="E22" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3916,8 +3985,11 @@
       <c r="E23" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3933,8 +4005,11 @@
       <c r="E24" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3950,8 +4025,11 @@
       <c r="E25" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3967,8 +4045,11 @@
       <c r="E26" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3984,8 +4065,11 @@
       <c r="E27" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4001,8 +4085,11 @@
       <c r="E28" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4018,8 +4105,11 @@
       <c r="E29" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4035,8 +4125,11 @@
       <c r="E30" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4052,8 +4145,11 @@
       <c r="E31" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4069,8 +4165,11 @@
       <c r="E32" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4086,8 +4185,11 @@
       <c r="E33" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4103,8 +4205,11 @@
       <c r="E34" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4120,8 +4225,11 @@
       <c r="E35" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4137,8 +4245,11 @@
       <c r="E36" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4154,8 +4265,11 @@
       <c r="E37" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4171,8 +4285,11 @@
       <c r="E38" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4188,8 +4305,11 @@
       <c r="E39" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4205,8 +4325,11 @@
       <c r="E40" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4222,8 +4345,11 @@
       <c r="E41" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4239,8 +4365,11 @@
       <c r="E42" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4256,8 +4385,11 @@
       <c r="E43" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4273,8 +4405,11 @@
       <c r="E44" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4290,8 +4425,11 @@
       <c r="E45" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4307,8 +4445,11 @@
       <c r="E46" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4324,8 +4465,11 @@
       <c r="E47" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F47">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4341,8 +4485,11 @@
       <c r="E48" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4358,8 +4505,11 @@
       <c r="E49" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4375,8 +4525,11 @@
       <c r="E50" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4392,8 +4545,11 @@
       <c r="E51" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F51">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4409,8 +4565,11 @@
       <c r="E52" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F52">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4426,8 +4585,11 @@
       <c r="E53" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F53">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4443,8 +4605,11 @@
       <c r="E54" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F54">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4460,8 +4625,11 @@
       <c r="E55" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F55">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4477,8 +4645,11 @@
       <c r="E56" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F56">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4494,8 +4665,11 @@
       <c r="E57" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F57">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4511,8 +4685,11 @@
       <c r="E58" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F58">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <f>A58+1</f>
         <v>58</v>
@@ -4529,8 +4706,11 @@
       <c r="E59" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F59">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" ref="A60:A123" si="0">A59+1</f>
         <v>59</v>
@@ -4547,8 +4727,11 @@
       <c r="E60" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -4565,8 +4748,11 @@
       <c r="E61" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F61">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -4583,8 +4769,11 @@
       <c r="E62" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F62">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -4601,8 +4790,11 @@
       <c r="E63" t="s">
         <v>918</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F63">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -4619,8 +4811,11 @@
       <c r="E64" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F64">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -4637,8 +4832,11 @@
       <c r="E65" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -4655,8 +4853,11 @@
       <c r="E66" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -4673,8 +4874,11 @@
       <c r="E67" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F67">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -4691,8 +4895,11 @@
       <c r="E68" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -4709,8 +4916,11 @@
       <c r="E69" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F69">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -4727,8 +4937,11 @@
       <c r="E70" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F70">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -4745,8 +4958,11 @@
       <c r="E71" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F71">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <f t="shared" si="0"/>
         <v>71</v>
@@ -4763,8 +4979,11 @@
       <c r="E72" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F72">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -4781,8 +5000,11 @@
       <c r="E73" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F73">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <f t="shared" si="0"/>
         <v>73</v>
@@ -4799,8 +5021,11 @@
       <c r="E74" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F74">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="0"/>
         <v>74</v>
@@ -4817,8 +5042,11 @@
       <c r="E75" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F75">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -4835,8 +5063,11 @@
       <c r="E76" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F76">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -4853,8 +5084,11 @@
       <c r="E77" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F77">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -4871,8 +5105,11 @@
       <c r="E78" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F78">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="0"/>
         <v>78</v>
@@ -4889,8 +5126,11 @@
       <c r="E79" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F79">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="0"/>
         <v>79</v>
@@ -4907,8 +5147,11 @@
       <c r="E80" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F80">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -4925,8 +5168,11 @@
       <c r="E81" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F81">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -4943,8 +5189,11 @@
       <c r="E82" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F82">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -4961,8 +5210,11 @@
       <c r="E83" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F83">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -4979,8 +5231,11 @@
       <c r="E84" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F84">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -4997,8 +5252,11 @@
       <c r="E85" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F85">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="0"/>
         <v>85</v>
@@ -5015,8 +5273,11 @@
       <c r="E86" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F86">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -5033,8 +5294,11 @@
       <c r="E87" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F87">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -5051,8 +5315,11 @@
       <c r="E88" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F88">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -5069,8 +5336,11 @@
       <c r="E89" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F89">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -5087,8 +5357,11 @@
       <c r="E90" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F90">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -5105,8 +5378,11 @@
       <c r="E91" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F91">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="0"/>
         <v>91</v>
@@ -5123,8 +5399,11 @@
       <c r="E92" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F92">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <f t="shared" si="0"/>
         <v>92</v>
@@ -5141,8 +5420,11 @@
       <c r="E93" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F93">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <f t="shared" si="0"/>
         <v>93</v>
@@ -5159,8 +5441,11 @@
       <c r="E94" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F94">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
         <f t="shared" si="0"/>
         <v>94</v>
@@ -5177,8 +5462,11 @@
       <c r="E95" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F95">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="0"/>
         <v>95</v>
@@ -5195,8 +5483,11 @@
       <c r="E96" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F96">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="0"/>
         <v>96</v>
@@ -5213,8 +5504,11 @@
       <c r="E97" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F97">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="0"/>
         <v>97</v>
@@ -5231,8 +5525,11 @@
       <c r="E98" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F98">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="0"/>
         <v>98</v>
@@ -5249,8 +5546,11 @@
       <c r="E99" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F99">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <f t="shared" si="0"/>
         <v>99</v>
@@ -5267,8 +5567,11 @@
       <c r="E100" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F100">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -5285,8 +5588,11 @@
       <c r="E101" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F101">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <f t="shared" si="0"/>
         <v>101</v>
@@ -5303,8 +5609,11 @@
       <c r="E102" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F102">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
         <f t="shared" si="0"/>
         <v>102</v>
@@ -5321,8 +5630,11 @@
       <c r="E103" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F103">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104">
         <f t="shared" si="0"/>
         <v>103</v>
@@ -5339,8 +5651,11 @@
       <c r="E104" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F104">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
         <f t="shared" si="0"/>
         <v>104</v>
@@ -5357,8 +5672,11 @@
       <c r="E105" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F105">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" si="0"/>
         <v>105</v>
@@ -5375,8 +5693,11 @@
       <c r="E106" t="s">
         <v>842</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F106">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107">
         <f t="shared" si="0"/>
         <v>106</v>
@@ -5393,8 +5714,11 @@
       <c r="E107" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F107">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108">
         <f t="shared" si="0"/>
         <v>107</v>
@@ -5411,8 +5735,11 @@
       <c r="E108" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F108" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109">
         <f t="shared" si="0"/>
         <v>108</v>
@@ -5429,8 +5756,11 @@
       <c r="E109" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F109">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110">
         <f t="shared" si="0"/>
         <v>109</v>
@@ -5447,8 +5777,11 @@
       <c r="E110" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F110">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111">
         <f t="shared" si="0"/>
         <v>110</v>
@@ -5465,8 +5798,11 @@
       <c r="E111" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F111">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112">
         <f t="shared" si="0"/>
         <v>111</v>
@@ -5483,8 +5819,11 @@
       <c r="E112" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F112">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113">
         <f t="shared" si="0"/>
         <v>112</v>
@@ -5501,8 +5840,11 @@
       <c r="E113" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F113">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114">
         <f t="shared" si="0"/>
         <v>113</v>
@@ -5519,8 +5861,11 @@
       <c r="E114" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F114">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115">
         <f t="shared" si="0"/>
         <v>114</v>
@@ -5537,8 +5882,11 @@
       <c r="E115" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F115">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116">
         <f t="shared" si="0"/>
         <v>115</v>
@@ -5555,8 +5903,11 @@
       <c r="E116" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F116">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117">
         <f t="shared" si="0"/>
         <v>116</v>
@@ -5573,8 +5924,11 @@
       <c r="E117" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F117">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118">
         <f t="shared" si="0"/>
         <v>117</v>
@@ -5591,8 +5945,11 @@
       <c r="E118" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F118">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119">
         <f t="shared" si="0"/>
         <v>118</v>
@@ -5609,8 +5966,11 @@
       <c r="E119" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F119">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120">
         <f t="shared" si="0"/>
         <v>119</v>
@@ -5627,8 +5987,11 @@
       <c r="E120" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F120">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121">
         <f t="shared" si="0"/>
         <v>120</v>
@@ -5645,8 +6008,11 @@
       <c r="E121" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F121">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122">
         <f t="shared" si="0"/>
         <v>121</v>
@@ -5663,8 +6029,11 @@
       <c r="E122" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F122">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123">
         <f t="shared" si="0"/>
         <v>122</v>
@@ -5681,8 +6050,11 @@
       <c r="E123" t="s">
         <v>984</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F123">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124">
         <f t="shared" ref="A124:A187" si="1">A123+1</f>
         <v>123</v>
@@ -5699,8 +6071,11 @@
       <c r="E124" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F124">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>124</v>
@@ -5717,8 +6092,11 @@
       <c r="E125" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F125">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -5735,8 +6113,11 @@
       <c r="E126" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F126">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>126</v>
@@ -5753,8 +6134,11 @@
       <c r="E127" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F127">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>127</v>
@@ -5771,8 +6155,11 @@
       <c r="E128" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F128">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129">
         <f t="shared" si="1"/>
         <v>128</v>
@@ -5789,8 +6176,11 @@
       <c r="E129" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F129">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -5807,8 +6197,11 @@
       <c r="E130" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F130">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -5825,8 +6218,11 @@
       <c r="E131" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F131">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132">
         <f t="shared" si="1"/>
         <v>131</v>
@@ -5843,8 +6239,11 @@
       <c r="E132" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F132">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133">
         <f t="shared" si="1"/>
         <v>132</v>
@@ -5861,8 +6260,11 @@
       <c r="E133" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F133">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134">
         <f t="shared" si="1"/>
         <v>133</v>
@@ -5879,8 +6281,11 @@
       <c r="E134" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F134">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135">
         <f t="shared" si="1"/>
         <v>134</v>
@@ -5897,8 +6302,11 @@
       <c r="E135" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F135">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136">
         <f t="shared" si="1"/>
         <v>135</v>
@@ -5915,8 +6323,11 @@
       <c r="E136" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F136">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137">
         <f t="shared" si="1"/>
         <v>136</v>
@@ -5933,8 +6344,11 @@
       <c r="E137" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F137">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138">
         <f t="shared" si="1"/>
         <v>137</v>
@@ -5951,8 +6365,11 @@
       <c r="E138" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F138">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139">
         <f t="shared" si="1"/>
         <v>138</v>
@@ -5969,8 +6386,11 @@
       <c r="E139" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F139">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140">
         <f t="shared" si="1"/>
         <v>139</v>
@@ -5987,8 +6407,11 @@
       <c r="E140" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F140">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -6005,8 +6428,11 @@
       <c r="E141" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F141">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142">
         <f t="shared" si="1"/>
         <v>141</v>
@@ -6023,8 +6449,11 @@
       <c r="E142" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F142">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143">
         <f t="shared" si="1"/>
         <v>142</v>
@@ -6041,8 +6470,11 @@
       <c r="E143" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F143">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144">
         <f t="shared" si="1"/>
         <v>143</v>
@@ -6059,8 +6491,11 @@
       <c r="E144" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F144">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145">
         <f t="shared" si="1"/>
         <v>144</v>
@@ -6077,8 +6512,11 @@
       <c r="E145" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F145">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146">
         <f t="shared" si="1"/>
         <v>145</v>
@@ -6095,8 +6533,11 @@
       <c r="E146" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F146">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147">
         <f t="shared" si="1"/>
         <v>146</v>
@@ -6113,8 +6554,11 @@
       <c r="E147" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F147">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148">
         <f t="shared" si="1"/>
         <v>147</v>
@@ -6131,8 +6575,11 @@
       <c r="E148" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F148">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149">
         <f t="shared" si="1"/>
         <v>148</v>
@@ -6149,8 +6596,11 @@
       <c r="E149" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F149">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150">
         <f t="shared" si="1"/>
         <v>149</v>
@@ -6167,8 +6617,11 @@
       <c r="E150" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F150">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151">
         <f t="shared" si="1"/>
         <v>150</v>
@@ -6185,8 +6638,11 @@
       <c r="E151" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F151">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152">
         <f t="shared" si="1"/>
         <v>151</v>
@@ -6203,8 +6659,11 @@
       <c r="E152" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F152">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153">
         <f t="shared" si="1"/>
         <v>152</v>
@@ -6221,8 +6680,11 @@
       <c r="E153" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F153">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154">
         <f t="shared" si="1"/>
         <v>153</v>
@@ -6239,8 +6701,11 @@
       <c r="E154" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F154">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155">
         <f t="shared" si="1"/>
         <v>154</v>
@@ -6257,8 +6722,11 @@
       <c r="E155" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F155">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156">
         <f t="shared" si="1"/>
         <v>155</v>
@@ -6275,8 +6743,11 @@
       <c r="E156" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F156">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157">
         <f t="shared" si="1"/>
         <v>156</v>
@@ -6293,8 +6764,11 @@
       <c r="E157" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F157">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158">
         <f t="shared" si="1"/>
         <v>157</v>
@@ -6311,8 +6785,11 @@
       <c r="E158" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F158">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159">
         <f t="shared" si="1"/>
         <v>158</v>
@@ -6329,8 +6806,11 @@
       <c r="E159" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F159">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160">
         <f t="shared" si="1"/>
         <v>159</v>
@@ -6347,8 +6827,11 @@
       <c r="E160" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F160">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161">
         <f t="shared" si="1"/>
         <v>160</v>
@@ -6365,8 +6848,11 @@
       <c r="E161" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F161">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162">
         <f t="shared" si="1"/>
         <v>161</v>
@@ -6383,8 +6869,11 @@
       <c r="E162" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F162">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163">
         <f t="shared" si="1"/>
         <v>162</v>
@@ -6401,8 +6890,11 @@
       <c r="E163" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F163">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164">
         <f t="shared" si="1"/>
         <v>163</v>
@@ -6419,8 +6911,11 @@
       <c r="E164" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F164">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165">
         <f t="shared" si="1"/>
         <v>164</v>
@@ -6437,8 +6932,11 @@
       <c r="E165" t="s">
         <v>833</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F165">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166">
         <f t="shared" si="1"/>
         <v>165</v>
@@ -6455,8 +6953,11 @@
       <c r="E166" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F166">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167">
         <f t="shared" si="1"/>
         <v>166</v>
@@ -6473,8 +6974,11 @@
       <c r="E167" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F167">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168">
         <f t="shared" si="1"/>
         <v>167</v>
@@ -6491,8 +6995,11 @@
       <c r="E168" t="s">
         <v>840</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F168">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169">
         <f t="shared" si="1"/>
         <v>168</v>
@@ -6509,8 +7016,11 @@
       <c r="E169" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F169">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170">
         <f t="shared" si="1"/>
         <v>169</v>
@@ -6527,8 +7037,11 @@
       <c r="E170" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F170">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171">
         <f t="shared" si="1"/>
         <v>170</v>
@@ -6545,8 +7058,11 @@
       <c r="E171" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F171">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172">
         <f t="shared" si="1"/>
         <v>171</v>
@@ -6563,8 +7079,11 @@
       <c r="E172" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F172">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173">
         <f t="shared" si="1"/>
         <v>172</v>
@@ -6581,8 +7100,11 @@
       <c r="E173" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F173">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174">
         <f t="shared" si="1"/>
         <v>173</v>
@@ -6599,8 +7121,11 @@
       <c r="E174" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F174">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175">
         <f t="shared" si="1"/>
         <v>174</v>
@@ -6617,8 +7142,11 @@
       <c r="E175" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F175">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176">
         <f t="shared" si="1"/>
         <v>175</v>
@@ -6635,8 +7163,11 @@
       <c r="E176" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F176">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177">
         <f t="shared" si="1"/>
         <v>176</v>
@@ -6653,8 +7184,11 @@
       <c r="E177" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F177">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178">
         <f t="shared" si="1"/>
         <v>177</v>
@@ -6671,8 +7205,11 @@
       <c r="E178" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F178">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179">
         <f t="shared" si="1"/>
         <v>178</v>
@@ -6689,8 +7226,11 @@
       <c r="E179" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F179">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180">
         <f t="shared" si="1"/>
         <v>179</v>
@@ -6707,8 +7247,11 @@
       <c r="E180" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F180">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181">
         <f t="shared" si="1"/>
         <v>180</v>
@@ -6725,8 +7268,11 @@
       <c r="E181" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F181">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182">
         <f t="shared" si="1"/>
         <v>181</v>
@@ -6743,8 +7289,11 @@
       <c r="E182" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F182">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183">
         <f t="shared" si="1"/>
         <v>182</v>
@@ -6761,8 +7310,11 @@
       <c r="E183" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F183">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184">
         <f t="shared" si="1"/>
         <v>183</v>
@@ -6779,8 +7331,11 @@
       <c r="E184" t="s">
         <v>869</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F184">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185">
         <f t="shared" si="1"/>
         <v>184</v>
@@ -6797,8 +7352,11 @@
       <c r="E185" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F185">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186">
         <f t="shared" si="1"/>
         <v>185</v>
@@ -6815,8 +7373,11 @@
       <c r="E186" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F186">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187">
         <f t="shared" si="1"/>
         <v>186</v>
@@ -6833,8 +7394,11 @@
       <c r="E187" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F187" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188">
         <f t="shared" ref="A188:A222" si="2">A187+1</f>
         <v>187</v>
@@ -6851,8 +7415,11 @@
       <c r="E188" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F188">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189">
         <f t="shared" si="2"/>
         <v>188</v>
@@ -6869,8 +7436,11 @@
       <c r="E189" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F189">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190">
         <f t="shared" si="2"/>
         <v>189</v>
@@ -6887,8 +7457,11 @@
       <c r="E190" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F190">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191">
         <f t="shared" si="2"/>
         <v>190</v>
@@ -6905,8 +7478,11 @@
       <c r="E191" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F191">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192">
         <f t="shared" si="2"/>
         <v>191</v>
@@ -6923,8 +7499,11 @@
       <c r="E192" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F192">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193">
         <f t="shared" si="2"/>
         <v>192</v>
@@ -6941,8 +7520,11 @@
       <c r="E193" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F193">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194">
         <f t="shared" si="2"/>
         <v>193</v>
@@ -6959,8 +7541,11 @@
       <c r="E194" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F194">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195">
         <f t="shared" si="2"/>
         <v>194</v>
@@ -6977,8 +7562,11 @@
       <c r="E195" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F195">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196">
         <f t="shared" si="2"/>
         <v>195</v>
@@ -6995,8 +7583,11 @@
       <c r="E196" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F196">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197">
         <f t="shared" si="2"/>
         <v>196</v>
@@ -7013,8 +7604,11 @@
       <c r="E197" t="s">
         <v>897</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F197">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198">
         <f t="shared" si="2"/>
         <v>197</v>
@@ -7031,8 +7625,11 @@
       <c r="E198" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F198">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199">
         <f t="shared" si="2"/>
         <v>198</v>
@@ -7049,8 +7646,11 @@
       <c r="E199" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F199">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200">
         <f t="shared" si="2"/>
         <v>199</v>
@@ -7067,8 +7667,11 @@
       <c r="E200" t="s">
         <v>905</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F200">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201">
         <f t="shared" si="2"/>
         <v>200</v>
@@ -7085,8 +7688,11 @@
       <c r="E201" t="s">
         <v>910</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F201">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202">
         <f t="shared" si="2"/>
         <v>201</v>
@@ -7103,8 +7709,11 @@
       <c r="E202" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F202">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203">
         <f t="shared" si="2"/>
         <v>202</v>
@@ -7121,8 +7730,11 @@
       <c r="E203" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F203">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204">
         <f t="shared" si="2"/>
         <v>203</v>
@@ -7139,8 +7751,11 @@
       <c r="E204" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F204" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205">
         <f t="shared" si="2"/>
         <v>204</v>
@@ -7157,8 +7772,11 @@
       <c r="E205" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F205">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206">
         <f t="shared" si="2"/>
         <v>205</v>
@@ -7175,8 +7793,11 @@
       <c r="E206" t="s">
         <v>914</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F206">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207">
         <f t="shared" si="2"/>
         <v>206</v>
@@ -7193,8 +7814,11 @@
       <c r="E207" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F207">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208">
         <f t="shared" si="2"/>
         <v>207</v>
@@ -7211,8 +7835,11 @@
       <c r="E208" t="s">
         <v>924</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F208">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209">
         <f t="shared" si="2"/>
         <v>208</v>
@@ -7229,8 +7856,11 @@
       <c r="E209" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F209">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210">
         <f t="shared" si="2"/>
         <v>209</v>
@@ -7247,8 +7877,11 @@
       <c r="E210" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F210">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A211">
         <f t="shared" si="2"/>
         <v>210</v>
@@ -7265,8 +7898,11 @@
       <c r="E211" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F211">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A212">
         <f t="shared" si="2"/>
         <v>211</v>
@@ -7283,8 +7919,11 @@
       <c r="E212" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F212">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A213">
         <f t="shared" si="2"/>
         <v>212</v>
@@ -7301,8 +7940,11 @@
       <c r="E213" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F213">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A214">
         <f t="shared" si="2"/>
         <v>213</v>
@@ -7319,8 +7961,11 @@
       <c r="E214" t="s">
         <v>867</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F214">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215">
         <f t="shared" si="2"/>
         <v>214</v>
@@ -7337,8 +7982,11 @@
       <c r="E215" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F215">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A216">
         <f t="shared" si="2"/>
         <v>215</v>
@@ -7355,8 +8003,11 @@
       <c r="E216" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F216">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A217">
         <f t="shared" si="2"/>
         <v>216</v>
@@ -7373,8 +8024,11 @@
       <c r="E217" t="s">
         <v>936</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F217">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A218">
         <f t="shared" si="2"/>
         <v>217</v>
@@ -7391,8 +8045,11 @@
       <c r="E218" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F218">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A219">
         <f t="shared" si="2"/>
         <v>218</v>
@@ -7409,8 +8066,11 @@
       <c r="E219" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F219">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A220">
         <f t="shared" si="2"/>
         <v>219</v>
@@ -7427,8 +8087,11 @@
       <c r="E220" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F220">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A221">
         <f t="shared" si="2"/>
         <v>220</v>
@@ -7445,8 +8108,11 @@
       <c r="E221" t="s">
         <v>939</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F221">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A222">
         <f t="shared" si="2"/>
         <v>221</v>
@@ -7462,6 +8128,9 @@
       </c>
       <c r="E222" t="s">
         <v>875</v>
+      </c>
+      <c r="F222">
+        <v>716</v>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.35">
@@ -7672,7 +8341,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D247:AK251 J2:AJ147 F148:AJ246 E2:E41 E43:E60 E177:E190 E63:E64 E74:E79 E81:E100 E102:E149 E202:E210 E151:E175 E239:E241 E213:E214 E192:E200 E66:E72 E216:E230 E232:E236 E243:E246 C2:C246 F2:F147">
+  <conditionalFormatting sqref="D247:AK251 J2:AJ147 F223:AJ246 E2:E41 E43:E60 E177:E190 E63:E64 E74:E79 E81:E100 E102:E149 E202:E210 E151:E175 E239:E241 E213:E214 E192:E200 E66:E72 E216:E230 E232:E236 E243:E246 C2:C246 G148:AJ222 F50 F60 F108 F187 F204">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -8607,8 +9276,8 @@
   </sheetPr>
   <dimension ref="A1:M267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E267"/>
+    <sheetView topLeftCell="A236" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D247" sqref="D247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
New confeeds functions introduced that automatically compile the R2S concordances from a small set of input concordances.
</commit_message>
<xml_diff>
--- a/ConcordanceLibrary/LabelsAndCodes/PIOLab_RootClassification.xlsx
+++ b/ConcordanceLibrary/LabelsAndCodes/PIOLab_RootClassification.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="1044">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -3160,6 +3160,9 @@
   </si>
   <si>
     <t>Limonite</t>
+  </si>
+  <si>
+    <t>Inputs from production-consumption system</t>
   </si>
 </sst>
 </file>
@@ -14071,7 +14074,7 @@
   <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14096,10 +14099,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1041</v>
-      </c>
-      <c r="C2" t="s">
-        <v>501</v>
+        <v>192</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1043</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -14107,7 +14110,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>1040</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>500</v>
@@ -14118,7 +14121,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1040</v>
+        <v>925</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>500</v>
@@ -14129,10 +14132,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>925</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>500</v>
+        <v>1041</v>
+      </c>
+      <c r="C5" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -14197,8 +14200,8 @@
       <c r="B11" t="s">
         <v>927</v>
       </c>
-      <c r="C11" t="s">
-        <v>501</v>
+      <c r="C11" s="4" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -14220,7 +14223,7 @@
         <v>504</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>500</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>